<commit_message>
clean up education datasets
</commit_message>
<xml_diff>
--- a/Datasets/college_complete_rural_urban_data/Overall_College_Complete_State.xlsx
+++ b/Datasets/college_complete_rural_urban_data/Overall_College_Complete_State.xlsx
@@ -5,20 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristanherink/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristanherink/Downloads/college_complete_rural_urban_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17899AB2-5908-AE4C-91E5-5277B38B1305}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4731A693-F93A-E845-90FF-ABED343E19F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{8643DEC3-34FF-6B45-9473-1B5731D3FDF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Alabama</t>
   </si>
@@ -182,9 +178,6 @@
   </si>
   <si>
     <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Puerto Rico</t>
   </si>
   <si>
     <t>State</t>
@@ -197,19 +190,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -245,13 +232,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -268,1079 +254,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1">
-            <v>1970</v>
-          </cell>
-          <cell r="C1">
-            <v>1980</v>
-          </cell>
-          <cell r="D1">
-            <v>1990</v>
-          </cell>
-          <cell r="E1">
-            <v>2000</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>2014-2018</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>8.8999999999999996E-2</v>
-          </cell>
-          <cell r="C2">
-            <v>0.13700000000000001</v>
-          </cell>
-          <cell r="D2">
-            <v>0.17799999999999999</v>
-          </cell>
-          <cell r="E2">
-            <v>0.217</v>
-          </cell>
-          <cell r="F2">
-            <v>0.28000000000000003</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0.155</v>
-          </cell>
-          <cell r="C3">
-            <v>0.22500000000000001</v>
-          </cell>
-          <cell r="D3">
-            <v>0.251</v>
-          </cell>
-          <cell r="E3">
-            <v>0.26600000000000001</v>
-          </cell>
-          <cell r="F3">
-            <v>0.318</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>0.13</v>
-          </cell>
-          <cell r="C4">
-            <v>0.17899999999999999</v>
-          </cell>
-          <cell r="D4">
-            <v>0.21</v>
-          </cell>
-          <cell r="E4">
-            <v>0.24199999999999999</v>
-          </cell>
-          <cell r="F4">
-            <v>0.29599999999999999</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>8.2000000000000003E-2</v>
-          </cell>
-          <cell r="C5">
-            <v>0.13300000000000001</v>
-          </cell>
-          <cell r="D5">
-            <v>0.16300000000000001</v>
-          </cell>
-          <cell r="E5">
-            <v>0.20200000000000001</v>
-          </cell>
-          <cell r="F5">
-            <v>0.26800000000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>0.13600000000000001</v>
-          </cell>
-          <cell r="C6">
-            <v>0.19700000000000001</v>
-          </cell>
-          <cell r="D6">
-            <v>0.23599999999999999</v>
-          </cell>
-          <cell r="E6">
-            <v>0.26800000000000002</v>
-          </cell>
-          <cell r="F6">
-            <v>0.33500000000000002</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0.16200000000000001</v>
-          </cell>
-          <cell r="C7">
-            <v>0.24</v>
-          </cell>
-          <cell r="D7">
-            <v>0.28199999999999997</v>
-          </cell>
-          <cell r="E7">
-            <v>0.34</v>
-          </cell>
-          <cell r="F7">
-            <v>0.41399999999999998</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0.13800000000000001</v>
-          </cell>
-          <cell r="C8">
-            <v>0.20799999999999999</v>
-          </cell>
-          <cell r="D8">
-            <v>0.27300000000000002</v>
-          </cell>
-          <cell r="E8">
-            <v>0.316</v>
-          </cell>
-          <cell r="F8">
-            <v>0.39200000000000002</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>0.13100000000000001</v>
-          </cell>
-          <cell r="C9">
-            <v>0.17499999999999999</v>
-          </cell>
-          <cell r="D9">
-            <v>0.214</v>
-          </cell>
-          <cell r="E9">
-            <v>0.25</v>
-          </cell>
-          <cell r="F9">
-            <v>0.314</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>0.17799999999999999</v>
-          </cell>
-          <cell r="C10">
-            <v>0.27500000000000002</v>
-          </cell>
-          <cell r="D10">
-            <v>0.33300000000000002</v>
-          </cell>
-          <cell r="E10">
-            <v>0.39100000000000001</v>
-          </cell>
-          <cell r="F10">
-            <v>0.57599999999999996</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>0.104</v>
-          </cell>
-          <cell r="C11">
-            <v>0.14799999999999999</v>
-          </cell>
-          <cell r="D11">
-            <v>0.186</v>
-          </cell>
-          <cell r="E11">
-            <v>0.22800000000000001</v>
-          </cell>
-          <cell r="F11">
-            <v>0.29699999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>0.106</v>
-          </cell>
-          <cell r="C12">
-            <v>0.16500000000000001</v>
-          </cell>
-          <cell r="D12">
-            <v>0.218</v>
-          </cell>
-          <cell r="E12">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F12">
-            <v>0.33700000000000002</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>0.15</v>
-          </cell>
-          <cell r="C13">
-            <v>0.21199999999999999</v>
-          </cell>
-          <cell r="D13">
-            <v>0.23799999999999999</v>
-          </cell>
-          <cell r="E13">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F13">
-            <v>0.33200000000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1">
-            <v>1970</v>
-          </cell>
-          <cell r="C1">
-            <v>1980</v>
-          </cell>
-          <cell r="D1">
-            <v>1990</v>
-          </cell>
-          <cell r="E1">
-            <v>2000</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>2014-2018</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>5.2999999999999999E-2</v>
-          </cell>
-          <cell r="C2">
-            <v>8.2000000000000003E-2</v>
-          </cell>
-          <cell r="D2">
-            <v>9.8000000000000004E-2</v>
-          </cell>
-          <cell r="E2">
-            <v>0.11600000000000001</v>
-          </cell>
-          <cell r="F2">
-            <v>0.152</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0.13500000000000001</v>
-          </cell>
-          <cell r="C3">
-            <v>0.189</v>
-          </cell>
-          <cell r="D3">
-            <v>0.192</v>
-          </cell>
-          <cell r="E3">
-            <v>0.21</v>
-          </cell>
-          <cell r="F3">
-            <v>0.23899999999999999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>7.4999999999999997E-2</v>
-          </cell>
-          <cell r="C4">
-            <v>0.10299999999999999</v>
-          </cell>
-          <cell r="D4">
-            <v>9.8000000000000004E-2</v>
-          </cell>
-          <cell r="E4">
-            <v>0.124</v>
-          </cell>
-          <cell r="F4">
-            <v>0.158</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>5.0999999999999997E-2</v>
-          </cell>
-          <cell r="C5">
-            <v>8.3000000000000004E-2</v>
-          </cell>
-          <cell r="D5">
-            <v>9.8000000000000004E-2</v>
-          </cell>
-          <cell r="E5">
-            <v>0.122</v>
-          </cell>
-          <cell r="F5">
-            <v>0.16</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>8.6999999999999994E-2</v>
-          </cell>
-          <cell r="C6">
-            <v>0.14599999999999999</v>
-          </cell>
-          <cell r="D6">
-            <v>0.156</v>
-          </cell>
-          <cell r="E6">
-            <v>0.18</v>
-          </cell>
-          <cell r="F6">
-            <v>0.23200000000000001</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>9.0999999999999998E-2</v>
-          </cell>
-          <cell r="C7">
-            <v>0.17199999999999999</v>
-          </cell>
-          <cell r="D7">
-            <v>0.19800000000000001</v>
-          </cell>
-          <cell r="E7">
-            <v>0.25</v>
-          </cell>
-          <cell r="F7">
-            <v>0.318</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0.12</v>
-          </cell>
-          <cell r="C8">
-            <v>0.186</v>
-          </cell>
-          <cell r="D8">
-            <v>0.25</v>
-          </cell>
-          <cell r="E8">
-            <v>0.27500000000000002</v>
-          </cell>
-          <cell r="F8">
-            <v>0.35099999999999998</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>6.2E-2</v>
-          </cell>
-          <cell r="C11">
-            <v>8.8999999999999996E-2</v>
-          </cell>
-          <cell r="D11">
-            <v>0.108</v>
-          </cell>
-          <cell r="E11">
-            <v>0.11799999999999999</v>
-          </cell>
-          <cell r="F11">
-            <v>0.14499999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>5.2999999999999999E-2</v>
-          </cell>
-          <cell r="C12">
-            <v>8.5000000000000006E-2</v>
-          </cell>
-          <cell r="D12">
-            <v>0.10100000000000001</v>
-          </cell>
-          <cell r="E12">
-            <v>0.125</v>
-          </cell>
-          <cell r="F12">
-            <v>0.16300000000000001</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>7.3999999999999996E-2</v>
-          </cell>
-          <cell r="C13">
-            <v>0.153</v>
-          </cell>
-          <cell r="D13">
-            <v>0.17799999999999999</v>
-          </cell>
-          <cell r="E13">
-            <v>0.21299999999999999</v>
-          </cell>
-          <cell r="F13">
-            <v>0.29499999999999998</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>8.5999999999999993E-2</v>
-          </cell>
-          <cell r="C14">
-            <v>0.14000000000000001</v>
-          </cell>
-          <cell r="D14">
-            <v>0.151</v>
-          </cell>
-          <cell r="E14">
-            <v>0.18</v>
-          </cell>
-          <cell r="F14">
-            <v>0.22500000000000001</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>6.0999999999999999E-2</v>
-          </cell>
-          <cell r="C15">
-            <v>9.5000000000000001E-2</v>
-          </cell>
-          <cell r="D15">
-            <v>0.11</v>
-          </cell>
-          <cell r="E15">
-            <v>0.13500000000000001</v>
-          </cell>
-          <cell r="F15">
-            <v>0.183</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>5.8000000000000003E-2</v>
-          </cell>
-          <cell r="C16">
-            <v>8.6999999999999994E-2</v>
-          </cell>
-          <cell r="D16">
-            <v>0.1</v>
-          </cell>
-          <cell r="E16">
-            <v>0.12</v>
-          </cell>
-          <cell r="F16">
-            <v>0.16400000000000001</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>6.9000000000000006E-2</v>
-          </cell>
-          <cell r="C17">
-            <v>0.107</v>
-          </cell>
-          <cell r="D17">
-            <v>0.125</v>
-          </cell>
-          <cell r="E17">
-            <v>0.155</v>
-          </cell>
-          <cell r="F17">
-            <v>0.20300000000000001</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>8.5999999999999993E-2</v>
-          </cell>
-          <cell r="C18">
-            <v>0.126</v>
-          </cell>
-          <cell r="D18">
-            <v>0.14499999999999999</v>
-          </cell>
-          <cell r="E18">
-            <v>0.17599999999999999</v>
-          </cell>
-          <cell r="F18">
-            <v>0.218</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>5.1999999999999998E-2</v>
-          </cell>
-          <cell r="C19">
-            <v>7.9000000000000001E-2</v>
-          </cell>
-          <cell r="D19">
-            <v>9.0999999999999998E-2</v>
-          </cell>
-          <cell r="E19">
-            <v>0.113</v>
-          </cell>
-          <cell r="F19">
-            <v>0.158</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>6.3E-2</v>
-          </cell>
-          <cell r="C20">
-            <v>9.2999999999999999E-2</v>
-          </cell>
-          <cell r="D20">
-            <v>0.10299999999999999</v>
-          </cell>
-          <cell r="E20">
-            <v>0.11899999999999999</v>
-          </cell>
-          <cell r="F20">
-            <v>0.14699999999999999</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>7.2999999999999995E-2</v>
-          </cell>
-          <cell r="C21">
-            <v>0.13200000000000001</v>
-          </cell>
-          <cell r="D21">
-            <v>0.16</v>
-          </cell>
-          <cell r="E21">
-            <v>0.19400000000000001</v>
-          </cell>
-          <cell r="F21">
-            <v>0.249</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>6.5000000000000002E-2</v>
-          </cell>
-          <cell r="C22">
-            <v>0.111</v>
-          </cell>
-          <cell r="D22">
-            <v>0.14299999999999999</v>
-          </cell>
-          <cell r="E22">
-            <v>0.17599999999999999</v>
-          </cell>
-          <cell r="F22">
-            <v>0.26100000000000001</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>0.108</v>
-          </cell>
-          <cell r="C23">
-            <v>0.19700000000000001</v>
-          </cell>
-          <cell r="D23">
-            <v>0.26</v>
-          </cell>
-          <cell r="E23">
-            <v>0.315</v>
-          </cell>
-          <cell r="F23">
-            <v>0.4</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>6.8000000000000005E-2</v>
-          </cell>
-          <cell r="C24">
-            <v>0.108</v>
-          </cell>
-          <cell r="D24">
-            <v>0.122</v>
-          </cell>
-          <cell r="E24">
-            <v>0.151</v>
-          </cell>
-          <cell r="F24">
-            <v>0.20699999999999999</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>6.7000000000000004E-2</v>
-          </cell>
-          <cell r="C25">
-            <v>0.108</v>
-          </cell>
-          <cell r="D25">
-            <v>0.128</v>
-          </cell>
-          <cell r="E25">
-            <v>0.16400000000000001</v>
-          </cell>
-          <cell r="F25">
-            <v>0.219</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-          <cell r="C26">
-            <v>0.105</v>
-          </cell>
-          <cell r="D26">
-            <v>0.123</v>
-          </cell>
-          <cell r="E26">
-            <v>0.14099999999999999</v>
-          </cell>
-          <cell r="F26">
-            <v>0.182</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>5.8000000000000003E-2</v>
-          </cell>
-          <cell r="C27">
-            <v>8.5999999999999993E-2</v>
-          </cell>
-          <cell r="D27">
-            <v>0.10199999999999999</v>
-          </cell>
-          <cell r="E27">
-            <v>0.125</v>
-          </cell>
-          <cell r="F27">
-            <v>0.16800000000000001</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>9.5000000000000001E-2</v>
-          </cell>
-          <cell r="C28">
-            <v>0.161</v>
-          </cell>
-          <cell r="D28">
-            <v>0.185</v>
-          </cell>
-          <cell r="E28">
-            <v>0.23100000000000001</v>
-          </cell>
-          <cell r="F28">
-            <v>0.3</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>6.7000000000000004E-2</v>
-          </cell>
-          <cell r="C29">
-            <v>0.114</v>
-          </cell>
-          <cell r="D29">
-            <v>0.13400000000000001</v>
-          </cell>
-          <cell r="E29">
-            <v>0.16900000000000001</v>
-          </cell>
-          <cell r="F29">
-            <v>0.221</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>8.2000000000000003E-2</v>
-          </cell>
-          <cell r="C30">
-            <v>0.121</v>
-          </cell>
-          <cell r="D30">
-            <v>0.129</v>
-          </cell>
-          <cell r="E30">
-            <v>0.14799999999999999</v>
-          </cell>
-          <cell r="F30">
-            <v>0.17599999999999999</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>0.106</v>
-          </cell>
-          <cell r="C31">
-            <v>0.17699999999999999</v>
-          </cell>
-          <cell r="D31">
-            <v>0.22500000000000001</v>
-          </cell>
-          <cell r="E31">
-            <v>0.26200000000000001</v>
-          </cell>
-          <cell r="F31">
-            <v>0.33400000000000002</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>0.10100000000000001</v>
-          </cell>
-          <cell r="C33">
-            <v>0.13500000000000001</v>
-          </cell>
-          <cell r="D33">
-            <v>0.14599999999999999</v>
-          </cell>
-          <cell r="E33">
-            <v>0.17199999999999999</v>
-          </cell>
-          <cell r="F33">
-            <v>0.19700000000000001</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>8.3000000000000004E-2</v>
-          </cell>
-          <cell r="C34">
-            <v>0.12</v>
-          </cell>
-          <cell r="D34">
-            <v>0.14299999999999999</v>
-          </cell>
-          <cell r="E34">
-            <v>0.16600000000000001</v>
-          </cell>
-          <cell r="F34">
-            <v>0.223</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>5.8000000000000003E-2</v>
-          </cell>
-          <cell r="C35">
-            <v>9.0999999999999998E-2</v>
-          </cell>
-          <cell r="D35">
-            <v>0.113</v>
-          </cell>
-          <cell r="E35">
-            <v>0.14299999999999999</v>
-          </cell>
-          <cell r="F35">
-            <v>0.193</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>6.4000000000000001E-2</v>
-          </cell>
-          <cell r="C36">
-            <v>0.11600000000000001</v>
-          </cell>
-          <cell r="D36">
-            <v>0.13900000000000001</v>
-          </cell>
-          <cell r="E36">
-            <v>0.17299999999999999</v>
-          </cell>
-          <cell r="F36">
-            <v>0.23300000000000001</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>6.0999999999999999E-2</v>
-          </cell>
-          <cell r="C37">
-            <v>9.1999999999999998E-2</v>
-          </cell>
-          <cell r="D37">
-            <v>0.104</v>
-          </cell>
-          <cell r="E37">
-            <v>0.126</v>
-          </cell>
-          <cell r="F37">
-            <v>0.16900000000000001</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>8.2000000000000003E-2</v>
-          </cell>
-          <cell r="C38">
-            <v>0.124</v>
-          </cell>
-          <cell r="D38">
-            <v>0.14299999999999999</v>
-          </cell>
-          <cell r="E38">
-            <v>0.16300000000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>0.19800000000000001</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="C39">
-            <v>0.122</v>
-          </cell>
-          <cell r="D39">
-            <v>0.13500000000000001</v>
-          </cell>
-          <cell r="E39">
-            <v>0.16</v>
-          </cell>
-          <cell r="F39">
-            <v>0.19600000000000001</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>5.5E-2</v>
-          </cell>
-          <cell r="C40">
-            <v>8.5999999999999993E-2</v>
-          </cell>
-          <cell r="D40">
-            <v>0.105</v>
-          </cell>
-          <cell r="E40">
-            <v>0.129</v>
-          </cell>
-          <cell r="F40">
-            <v>0.17899999999999999</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>6.8000000000000005E-2</v>
-          </cell>
-          <cell r="C42">
-            <v>9.9000000000000005E-2</v>
-          </cell>
-          <cell r="D42">
-            <v>0.114</v>
-          </cell>
-          <cell r="E42">
-            <v>0.13900000000000001</v>
-          </cell>
-          <cell r="F42">
-            <v>0.17499999999999999</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>8.2000000000000003E-2</v>
-          </cell>
-          <cell r="C43">
-            <v>0.13</v>
-          </cell>
-          <cell r="D43">
-            <v>0.155</v>
-          </cell>
-          <cell r="E43">
-            <v>0.193</v>
-          </cell>
-          <cell r="F43">
-            <v>0.254</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>4.4999999999999998E-2</v>
-          </cell>
-          <cell r="C44">
-            <v>7.3999999999999996E-2</v>
-          </cell>
-          <cell r="D44">
-            <v>8.7999999999999995E-2</v>
-          </cell>
-          <cell r="E44">
-            <v>0.11</v>
-          </cell>
-          <cell r="F44">
-            <v>0.155</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>6.9000000000000006E-2</v>
-          </cell>
-          <cell r="C45">
-            <v>0.10199999999999999</v>
-          </cell>
-          <cell r="D45">
-            <v>0.115</v>
-          </cell>
-          <cell r="E45">
-            <v>0.13500000000000001</v>
-          </cell>
-          <cell r="F45">
-            <v>0.16700000000000001</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>9.4E-2</v>
-          </cell>
-          <cell r="C46">
-            <v>0.14099999999999999</v>
-          </cell>
-          <cell r="D46">
-            <v>0.159</v>
-          </cell>
-          <cell r="E46">
-            <v>0.20899999999999999</v>
-          </cell>
-          <cell r="F46">
-            <v>0.27100000000000002</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>0.104</v>
-          </cell>
-          <cell r="C47">
-            <v>0.17799999999999999</v>
-          </cell>
-          <cell r="D47">
-            <v>0.223</v>
-          </cell>
-          <cell r="E47">
-            <v>0.27</v>
-          </cell>
-          <cell r="F47">
-            <v>0.34</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>5.1999999999999998E-2</v>
-          </cell>
-          <cell r="C48">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="D48">
-            <v>9.7000000000000003E-2</v>
-          </cell>
-          <cell r="E48">
-            <v>0.124</v>
-          </cell>
-          <cell r="F48">
-            <v>0.17399999999999999</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>0.10100000000000001</v>
-          </cell>
-          <cell r="C49">
-            <v>0.14699999999999999</v>
-          </cell>
-          <cell r="D49">
-            <v>0.16400000000000001</v>
-          </cell>
-          <cell r="E49">
-            <v>0.19800000000000001</v>
-          </cell>
-          <cell r="F49">
-            <v>0.251</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>5.3999999999999999E-2</v>
-          </cell>
-          <cell r="C50">
-            <v>8.4000000000000005E-2</v>
-          </cell>
-          <cell r="D50">
-            <v>9.5000000000000001E-2</v>
-          </cell>
-          <cell r="E50">
-            <v>0.115</v>
-          </cell>
-          <cell r="F50">
-            <v>0.16</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>6.7000000000000004E-2</v>
-          </cell>
-          <cell r="C51">
-            <v>0.108</v>
-          </cell>
-          <cell r="D51">
-            <v>0.124</v>
-          </cell>
-          <cell r="E51">
-            <v>0.156</v>
-          </cell>
-          <cell r="F51">
-            <v>0.21199999999999999</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>0.111</v>
-          </cell>
-          <cell r="C52">
-            <v>0.16500000000000001</v>
-          </cell>
-          <cell r="D52">
-            <v>0.18</v>
-          </cell>
-          <cell r="E52">
-            <v>0.219</v>
-          </cell>
-          <cell r="F52">
-            <v>0.27300000000000002</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="E53">
-            <v>0.122</v>
-          </cell>
-          <cell r="F53">
-            <v>0.193</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1640,17 +553,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3F9DC2-BD3A-8146-AC22-D1A40B858964}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1">
         <v>1970</v>
@@ -1665,7 +578,7 @@
         <v>2000</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2608,7 +1521,7 @@
         <v>0.38200000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -2628,7 +1541,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -2648,7 +1561,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2668,7 +1581,7 @@
         <v>0.29499999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -2688,83 +1601,59 @@
         <v>0.26900000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="2">
-        <v>0.183</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0.253</v>
-      </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="2">
-        <v>0.185</v>
-      </c>
-      <c r="K53" s="2">
-        <v>0.25600000000000001</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" xr:uid="{52F53D40-C8AE-6B4C-A323-DDBAA0E00AAD}"/>
-    <hyperlink ref="A3" xr:uid="{DB0E1EC8-F582-DA40-8BEB-3DC4B18EFBC1}"/>
-    <hyperlink ref="A4" xr:uid="{F3E50100-4228-4E46-93CD-39E229A08B5D}"/>
-    <hyperlink ref="A5" xr:uid="{AB5FBF5A-F704-7045-9B50-EFBD5891932C}"/>
-    <hyperlink ref="A6" xr:uid="{0426F934-62A2-2043-B905-BDDE2A94E959}"/>
-    <hyperlink ref="A7" xr:uid="{77C51493-1935-684D-BCD3-421C744D281D}"/>
-    <hyperlink ref="A8" xr:uid="{CAEB3213-00A9-904A-9152-7CC51AB52284}"/>
-    <hyperlink ref="A9" xr:uid="{A3708330-3712-2E4A-B515-F95636C89B61}"/>
-    <hyperlink ref="A10" xr:uid="{9AEE5513-CA95-524B-9D49-E1BCBA13CBE2}"/>
-    <hyperlink ref="A11" xr:uid="{A66BBE53-3566-6C49-87A3-942A703CC2B8}"/>
-    <hyperlink ref="A12" xr:uid="{5FB6105A-57F6-FF4D-AAEA-5BAB51D3817A}"/>
-    <hyperlink ref="A13" xr:uid="{1C3315FF-9050-8A4C-B82B-AED86676A83D}"/>
-    <hyperlink ref="A14" xr:uid="{19C0D461-51C2-5445-A3E2-AF3243557A5E}"/>
-    <hyperlink ref="A15" xr:uid="{002BF7AE-CCA3-2942-BE68-7EBB61AC1A9C}"/>
-    <hyperlink ref="A16" xr:uid="{2D5F7759-B0B8-274E-B359-653D7C6A8C95}"/>
-    <hyperlink ref="A17" xr:uid="{7E8FE43C-85AB-3A4A-AFAE-18CF8A350D8A}"/>
-    <hyperlink ref="A18" xr:uid="{4070082A-B4DC-BA4C-AD1E-AFA97D809A4D}"/>
-    <hyperlink ref="A19" xr:uid="{EB3F2D81-178F-3047-A60C-C41A20A0C7A8}"/>
-    <hyperlink ref="A20" xr:uid="{3835DA88-6EEB-E547-9B3E-DD671ACF5385}"/>
-    <hyperlink ref="A21" xr:uid="{DB2AAC52-D864-254A-8DA8-375FD0D7E948}"/>
-    <hyperlink ref="A22" xr:uid="{16E701F1-7C21-094D-83CC-9B6EC821B391}"/>
-    <hyperlink ref="A23" xr:uid="{FD4004AE-C44A-A149-AE49-D5FBB541D532}"/>
-    <hyperlink ref="A24" xr:uid="{31F8AAA1-E121-3B49-91C8-EF9F7096C43F}"/>
-    <hyperlink ref="A25" xr:uid="{528DEF7A-00BF-5A4B-B970-74F75D040C07}"/>
-    <hyperlink ref="A26" xr:uid="{15CCF40F-9787-7A40-ABFE-89DF3E1FE3B4}"/>
-    <hyperlink ref="A27" xr:uid="{6CC080A2-0FBE-174F-B193-DEFD94E47BE3}"/>
-    <hyperlink ref="A28" xr:uid="{72CDF7DB-A639-7E48-92FE-6B865316C2AF}"/>
-    <hyperlink ref="A29" xr:uid="{7F5AD59E-FD6A-404E-BFE2-DA3963504B1A}"/>
-    <hyperlink ref="A30" xr:uid="{4031DA3F-651B-1C46-AE72-42BF0006348E}"/>
-    <hyperlink ref="A31" xr:uid="{966772B0-8CC7-D442-ADE3-7AC43FDA7C52}"/>
-    <hyperlink ref="A32" xr:uid="{1AD067B1-5B3E-D042-BD1A-58CF9145E8C9}"/>
-    <hyperlink ref="A33" xr:uid="{7065D618-90AC-524C-82D5-FD6FF00CE2A5}"/>
-    <hyperlink ref="A34" xr:uid="{B6DB5778-41DE-AA4C-BE49-BAE7EA765A35}"/>
-    <hyperlink ref="A35" xr:uid="{8E30D3DC-0564-1F43-8AC7-DC7D0E67C054}"/>
-    <hyperlink ref="A36" xr:uid="{49BB0E28-A2DE-D74F-A988-615368BE883F}"/>
-    <hyperlink ref="A37" xr:uid="{567B51A3-52B2-3C45-A078-62EBD0BCAA95}"/>
-    <hyperlink ref="A38" xr:uid="{A5BD42E3-C5E7-E44F-84E5-FE33208ADEEC}"/>
-    <hyperlink ref="A39" xr:uid="{BE42ECF0-1A27-1041-A659-B769493C095F}"/>
-    <hyperlink ref="A40" xr:uid="{DDDA02BC-F01F-9841-A12D-F625758A55C6}"/>
-    <hyperlink ref="A41" xr:uid="{43A4F9DA-4694-7B4F-8B71-3EAF1C3AF489}"/>
-    <hyperlink ref="A42" xr:uid="{67C2E5AD-B9EA-DE40-8B19-1E71B7363C59}"/>
-    <hyperlink ref="A43" xr:uid="{3D5B8E97-F4F9-0D4F-8B9D-06C5B470380A}"/>
-    <hyperlink ref="A44" xr:uid="{640AF17E-64C2-BC42-9D9E-3C9E2E7EAA23}"/>
-    <hyperlink ref="A45" xr:uid="{26B4C7E7-1A9E-5843-BB54-29153E19DB0C}"/>
-    <hyperlink ref="A46" xr:uid="{AFAEE757-F71B-9E46-993D-EB0F30153654}"/>
-    <hyperlink ref="A47" xr:uid="{61A5F792-54B3-0446-AD94-50989C49B1EB}"/>
-    <hyperlink ref="A48" xr:uid="{E1065C53-6F46-9044-A702-7901169385ED}"/>
-    <hyperlink ref="A49" xr:uid="{7D3A5424-A3FA-8048-9401-550DC9C2323B}"/>
-    <hyperlink ref="A50" xr:uid="{1D038DC0-6369-6644-9E9B-6700E14258E3}"/>
-    <hyperlink ref="A51" xr:uid="{3C5F6D72-223F-7D45-A22B-9D61250D26E7}"/>
-    <hyperlink ref="A52" xr:uid="{8F6D4C5C-9CA7-3940-A68B-17B7348CF237}"/>
-    <hyperlink ref="A53" xr:uid="{D79EE8FB-583E-E84C-847C-AAD7F8D7A6EC}"/>
+    <hyperlink ref="A2" display="Alabama" xr:uid="{52F53D40-C8AE-6B4C-A323-DDBAA0E00AAD}"/>
+    <hyperlink ref="A3" display="Alaska" xr:uid="{DB0E1EC8-F582-DA40-8BEB-3DC4B18EFBC1}"/>
+    <hyperlink ref="A4" display="Arizona" xr:uid="{F3E50100-4228-4E46-93CD-39E229A08B5D}"/>
+    <hyperlink ref="A5" display="Arkansas" xr:uid="{AB5FBF5A-F704-7045-9B50-EFBD5891932C}"/>
+    <hyperlink ref="A6" display="California" xr:uid="{0426F934-62A2-2043-B905-BDDE2A94E959}"/>
+    <hyperlink ref="A7" display="Colorado" xr:uid="{77C51493-1935-684D-BCD3-421C744D281D}"/>
+    <hyperlink ref="A8" display="Connecticut" xr:uid="{CAEB3213-00A9-904A-9152-7CC51AB52284}"/>
+    <hyperlink ref="A9" display="Delaware" xr:uid="{A3708330-3712-2E4A-B515-F95636C89B61}"/>
+    <hyperlink ref="A10" display="District of Columbia" xr:uid="{9AEE5513-CA95-524B-9D49-E1BCBA13CBE2}"/>
+    <hyperlink ref="A11" display="Florida" xr:uid="{A66BBE53-3566-6C49-87A3-942A703CC2B8}"/>
+    <hyperlink ref="A12" display="Georgia" xr:uid="{5FB6105A-57F6-FF4D-AAEA-5BAB51D3817A}"/>
+    <hyperlink ref="A13" display="Hawaii" xr:uid="{1C3315FF-9050-8A4C-B82B-AED86676A83D}"/>
+    <hyperlink ref="A14" display="Idaho" xr:uid="{19C0D461-51C2-5445-A3E2-AF3243557A5E}"/>
+    <hyperlink ref="A15" display="Illinois" xr:uid="{002BF7AE-CCA3-2942-BE68-7EBB61AC1A9C}"/>
+    <hyperlink ref="A16" display="Indiana" xr:uid="{2D5F7759-B0B8-274E-B359-653D7C6A8C95}"/>
+    <hyperlink ref="A17" display="Iowa" xr:uid="{7E8FE43C-85AB-3A4A-AFAE-18CF8A350D8A}"/>
+    <hyperlink ref="A18" display="Kansas" xr:uid="{4070082A-B4DC-BA4C-AD1E-AFA97D809A4D}"/>
+    <hyperlink ref="A19" display="Kentucky" xr:uid="{EB3F2D81-178F-3047-A60C-C41A20A0C7A8}"/>
+    <hyperlink ref="A20" display="Louisiana" xr:uid="{3835DA88-6EEB-E547-9B3E-DD671ACF5385}"/>
+    <hyperlink ref="A21" display="Maine" xr:uid="{DB2AAC52-D864-254A-8DA8-375FD0D7E948}"/>
+    <hyperlink ref="A22" display="Maryland" xr:uid="{16E701F1-7C21-094D-83CC-9B6EC821B391}"/>
+    <hyperlink ref="A23" display="Massachusetts" xr:uid="{FD4004AE-C44A-A149-AE49-D5FBB541D532}"/>
+    <hyperlink ref="A24" display="Michigan" xr:uid="{31F8AAA1-E121-3B49-91C8-EF9F7096C43F}"/>
+    <hyperlink ref="A25" display="Minnesota" xr:uid="{528DEF7A-00BF-5A4B-B970-74F75D040C07}"/>
+    <hyperlink ref="A26" display="Mississippi" xr:uid="{15CCF40F-9787-7A40-ABFE-89DF3E1FE3B4}"/>
+    <hyperlink ref="A27" display="Missouri" xr:uid="{6CC080A2-0FBE-174F-B193-DEFD94E47BE3}"/>
+    <hyperlink ref="A28" display="Montana" xr:uid="{72CDF7DB-A639-7E48-92FE-6B865316C2AF}"/>
+    <hyperlink ref="A29" display="Nebraska" xr:uid="{7F5AD59E-FD6A-404E-BFE2-DA3963504B1A}"/>
+    <hyperlink ref="A30" display="Nevada" xr:uid="{4031DA3F-651B-1C46-AE72-42BF0006348E}"/>
+    <hyperlink ref="A31" display="New Hampshire" xr:uid="{966772B0-8CC7-D442-ADE3-7AC43FDA7C52}"/>
+    <hyperlink ref="A32" display="New Jersey" xr:uid="{1AD067B1-5B3E-D042-BD1A-58CF9145E8C9}"/>
+    <hyperlink ref="A33" display="New Mexico" xr:uid="{7065D618-90AC-524C-82D5-FD6FF00CE2A5}"/>
+    <hyperlink ref="A34" display="New York" xr:uid="{B6DB5778-41DE-AA4C-BE49-BAE7EA765A35}"/>
+    <hyperlink ref="A35" display="North Carolina" xr:uid="{8E30D3DC-0564-1F43-8AC7-DC7D0E67C054}"/>
+    <hyperlink ref="A36" display="North Dakota" xr:uid="{49BB0E28-A2DE-D74F-A988-615368BE883F}"/>
+    <hyperlink ref="A37" display="Ohio" xr:uid="{567B51A3-52B2-3C45-A078-62EBD0BCAA95}"/>
+    <hyperlink ref="A38" display="Oklahoma" xr:uid="{A5BD42E3-C5E7-E44F-84E5-FE33208ADEEC}"/>
+    <hyperlink ref="A39" display="Oregon" xr:uid="{BE42ECF0-1A27-1041-A659-B769493C095F}"/>
+    <hyperlink ref="A40" display="Pennsylvania" xr:uid="{DDDA02BC-F01F-9841-A12D-F625758A55C6}"/>
+    <hyperlink ref="A41" display="Rhode Island" xr:uid="{43A4F9DA-4694-7B4F-8B71-3EAF1C3AF489}"/>
+    <hyperlink ref="A42" display="South Carolina" xr:uid="{67C2E5AD-B9EA-DE40-8B19-1E71B7363C59}"/>
+    <hyperlink ref="A43" display="South Dakota" xr:uid="{3D5B8E97-F4F9-0D4F-8B9D-06C5B470380A}"/>
+    <hyperlink ref="A44" display="Tennessee" xr:uid="{640AF17E-64C2-BC42-9D9E-3C9E2E7EAA23}"/>
+    <hyperlink ref="A45" display="Texas" xr:uid="{26B4C7E7-1A9E-5843-BB54-29153E19DB0C}"/>
+    <hyperlink ref="A46" display="Utah" xr:uid="{AFAEE757-F71B-9E46-993D-EB0F30153654}"/>
+    <hyperlink ref="A47" display="Vermont" xr:uid="{61A5F792-54B3-0446-AD94-50989C49B1EB}"/>
+    <hyperlink ref="A48" display="Virginia" xr:uid="{E1065C53-6F46-9044-A702-7901169385ED}"/>
+    <hyperlink ref="A49" display="Washington" xr:uid="{7D3A5424-A3FA-8048-9401-550DC9C2323B}"/>
+    <hyperlink ref="A50" display="West Virginia" xr:uid="{1D038DC0-6369-6644-9E9B-6700E14258E3}"/>
+    <hyperlink ref="A51" display="Wisconsin" xr:uid="{3C5F6D72-223F-7D45-A22B-9D61250D26E7}"/>
+    <hyperlink ref="A52" display="Wyoming" xr:uid="{8F6D4C5C-9CA7-3940-A68B-17B7348CF237}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>